<commit_message>
Modify data for testing purposes
</commit_message>
<xml_diff>
--- a/DSEC/base/data/Configuration_Audit.xlsx
+++ b/DSEC/base/data/Configuration_Audit.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geors\Documents\Defsecone\Products\DSEC360+\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Defsecone\DSEC360-Backend\DSEC\base\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B50D8B5-D946-4C92-9F83-372CEFFE8186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37E52D-01FB-41D0-933D-9909C6307AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$65</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -423,20 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -469,18 +469,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -488,10 +488,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -499,21 +499,21 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -521,32 +521,32 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -554,10 +554,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -565,21 +565,21 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -587,21 +587,21 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -609,10 +609,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -620,21 +620,21 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -642,10 +642,10 @@
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -653,21 +653,21 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -675,21 +675,21 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -697,10 +697,10 @@
         <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -708,21 +708,21 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -730,10 +730,10 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -741,21 +741,21 @@
         <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -763,21 +763,21 @@
         <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -785,10 +785,10 @@
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -796,21 +796,21 @@
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -818,10 +818,10 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -829,21 +829,21 @@
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -851,21 +851,21 @@
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -873,10 +873,10 @@
         <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -884,21 +884,21 @@
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -906,10 +906,10 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -917,21 +917,21 @@
         <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -939,21 +939,21 @@
         <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -961,10 +961,10 @@
         <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -972,21 +972,21 @@
         <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -994,10 +994,10 @@
         <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -1005,21 +1005,21 @@
         <v>16</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>22</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -1027,21 +1027,21 @@
         <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -1049,10 +1049,10 @@
         <v>18</v>
       </c>
       <c r="C56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -1060,21 +1060,21 @@
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -1082,10 +1082,10 @@
         <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -1093,21 +1093,21 @@
         <v>16</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -1115,21 +1115,21 @@
         <v>17</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -1137,10 +1137,10 @@
         <v>18</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -1148,17 +1148,6 @@
         <v>18</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>23</v>
-      </c>
-      <c r="B66" t="s">
-        <v>18</v>
-      </c>
-      <c r="C66" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>